<commit_message>
Commit: Create data - Student preferences created based on gaussian distribution of project popularity
</commit_message>
<xml_diff>
--- a/Staff&Projects(60).xlsx
+++ b/Staff&Projects(60).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="123">
   <si>
     <t>Supervisor</t>
   </si>
@@ -23,49 +23,127 @@
     <t>Target Audience</t>
   </si>
   <si>
-    <t>Edward Hopper</t>
-  </si>
-  <si>
-    <t>painting melancholy pictures</t>
+    <t>Wile E. Coyote</t>
+  </si>
+  <si>
+    <t>testing new technologies</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>Abstract views on testing new technologies</t>
+  </si>
+  <si>
+    <t>Ozzy Osbourne</t>
+  </si>
+  <si>
+    <t>singing rock songs</t>
+  </si>
+  <si>
+    <t>CS</t>
+  </si>
+  <si>
+    <t>writing rock songs</t>
   </si>
   <si>
     <t>CS + DS</t>
   </si>
   <si>
-    <t>Abstract views on painting melancholy pictures</t>
-  </si>
-  <si>
-    <t>CS</t>
-  </si>
-  <si>
-    <t>Confucius</t>
-  </si>
-  <si>
-    <t>teaching philosophy</t>
-  </si>
-  <si>
-    <t>spreading philosophy</t>
-  </si>
-  <si>
-    <t>teaching the next generation</t>
-  </si>
-  <si>
-    <t>Princess Leia Organa</t>
-  </si>
-  <si>
-    <t>leading the rebel alliance</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>smuggling military plans</t>
-  </si>
-  <si>
-    <t>Abstract views on leading the rebel alliance</t>
-  </si>
-  <si>
-    <t>Matt Drudge</t>
+    <t>Abstract views on singing rock songs</t>
+  </si>
+  <si>
+    <t>Edward Cullen</t>
+  </si>
+  <si>
+    <t>sucking blood</t>
+  </si>
+  <si>
+    <t>avoiding growing old</t>
+  </si>
+  <si>
+    <t>Abstract views on sucking blood</t>
+  </si>
+  <si>
+    <t>Ella Fitzgerald</t>
+  </si>
+  <si>
+    <t>singing torch songs</t>
+  </si>
+  <si>
+    <t>singing the blues</t>
+  </si>
+  <si>
+    <t>Abstract views on singing torch songs</t>
+  </si>
+  <si>
+    <t>Indiana Jones</t>
+  </si>
+  <si>
+    <t>looking for hidden treasures</t>
+  </si>
+  <si>
+    <t>punching out Nazis</t>
+  </si>
+  <si>
+    <t>digging for antiquities</t>
+  </si>
+  <si>
+    <t>unearthing ancient tombs</t>
+  </si>
+  <si>
+    <t>Babe Ruth</t>
+  </si>
+  <si>
+    <t>hitting home runs</t>
+  </si>
+  <si>
+    <t>Abstract views on hitting home runs</t>
+  </si>
+  <si>
+    <t>James Joyce</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>Abstract views on writing modern fiction</t>
+  </si>
+  <si>
+    <t>Edmund Blackadder</t>
+  </si>
+  <si>
+    <t>manipulating political pawns</t>
+  </si>
+  <si>
+    <t>climbing social ladders</t>
+  </si>
+  <si>
+    <t>wielding political power</t>
+  </si>
+  <si>
+    <t>Steve Jobs</t>
+  </si>
+  <si>
+    <t>running a software company</t>
+  </si>
+  <si>
+    <t>running a technology company</t>
+  </si>
+  <si>
+    <t>running a hardware company</t>
+  </si>
+  <si>
+    <t>pioneering new technologies</t>
+  </si>
+  <si>
+    <t>terrorizing employees</t>
+  </si>
+  <si>
+    <t xml:space="preserve">developing new technologies </t>
+  </si>
+  <si>
+    <t>Stephen Colbert</t>
   </si>
   <si>
     <t>promoting conservative values</t>
@@ -74,28 +152,94 @@
     <t>ranting about liberals</t>
   </si>
   <si>
-    <t>spreading political gossip</t>
-  </si>
-  <si>
-    <t>Jamie Oliver</t>
-  </si>
-  <si>
-    <t>cooking dinners</t>
-  </si>
-  <si>
-    <t>running restaurants</t>
-  </si>
-  <si>
-    <t>promoting healthy eating</t>
-  </si>
-  <si>
-    <t>Mr. Bean</t>
-  </si>
-  <si>
-    <t>causing mayhem</t>
-  </si>
-  <si>
-    <t>Abstract views on causing mayhem</t>
+    <t>Abstract views on promoting conservative values</t>
+  </si>
+  <si>
+    <t>Tony Stark</t>
+  </si>
+  <si>
+    <t>running a multinational corporation</t>
+  </si>
+  <si>
+    <t>Leroy Jethro Gibbs</t>
+  </si>
+  <si>
+    <t>solving mysteries</t>
+  </si>
+  <si>
+    <t>solving crimes</t>
+  </si>
+  <si>
+    <t>finding clues</t>
+  </si>
+  <si>
+    <t>interpreting evidence</t>
+  </si>
+  <si>
+    <t>Aung San Suu Kyi</t>
+  </si>
+  <si>
+    <t>campaigning for democracy</t>
+  </si>
+  <si>
+    <t>Abstract views on campaigning for democracy</t>
+  </si>
+  <si>
+    <t>Al Pacino</t>
+  </si>
+  <si>
+    <t>shouting in Hollywood movies</t>
+  </si>
+  <si>
+    <t>Abstract views on shouting in Hollywood movies</t>
+  </si>
+  <si>
+    <t>George Clooney</t>
+  </si>
+  <si>
+    <t>starring in Hollywood movies</t>
+  </si>
+  <si>
+    <t>starring in indy movies</t>
+  </si>
+  <si>
+    <t>womanizing</t>
+  </si>
+  <si>
+    <t>promoting political causes</t>
+  </si>
+  <si>
+    <t>Coco Chanel</t>
+  </si>
+  <si>
+    <t>designing haute couture</t>
+  </si>
+  <si>
+    <t>selling perfumes</t>
+  </si>
+  <si>
+    <t>Abstract views on designing haute couture</t>
+  </si>
+  <si>
+    <t>George Costanza</t>
+  </si>
+  <si>
+    <t>complaining about life</t>
+  </si>
+  <si>
+    <t>Abstract views on complaining about life</t>
+  </si>
+  <si>
+    <t>Cher</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>Abstract views on singing pop songs</t>
   </si>
   <si>
     <t>Bernard Madoff</t>
@@ -110,256 +254,133 @@
     <t>running pyramid schemes</t>
   </si>
   <si>
-    <t>Robert Langdon</t>
-  </si>
-  <si>
-    <t>studying symbols</t>
-  </si>
-  <si>
-    <t>studying icons</t>
-  </si>
-  <si>
-    <t>following clues</t>
-  </si>
-  <si>
-    <t>Reince Priebus</t>
-  </si>
-  <si>
-    <t>Abstract views on promoting conservative values</t>
-  </si>
-  <si>
-    <t>Jim Morrison</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>writing rock songs</t>
-  </si>
-  <si>
-    <t>Abstract views on singing rock songs</t>
-  </si>
-  <si>
-    <t>Morpheus</t>
-  </si>
-  <si>
-    <t>searching for the messiah</t>
-  </si>
-  <si>
-    <t>recruiting dissidents</t>
-  </si>
-  <si>
-    <t>raging against the machine</t>
-  </si>
-  <si>
-    <t>Dorian Gray</t>
-  </si>
-  <si>
-    <t>gadding about town</t>
-  </si>
-  <si>
-    <t>practicing good skin care</t>
-  </si>
-  <si>
-    <t>avoiding growing old</t>
-  </si>
-  <si>
-    <t>Tony Robbins</t>
-  </si>
-  <si>
-    <t>selling self-help books</t>
-  </si>
-  <si>
-    <t>giving self-help lectures,</t>
-  </si>
-  <si>
-    <t>Abstract views on selling self-help books</t>
-  </si>
-  <si>
-    <t>Conan the Barbarian</t>
-  </si>
-  <si>
-    <t>stealing jewels</t>
-  </si>
-  <si>
-    <t>fighting barbarian hordes</t>
-  </si>
-  <si>
-    <t>defending the weak</t>
+    <t>Deadpool</t>
   </si>
   <si>
     <t>foiling the schemes of evil villains</t>
   </si>
   <si>
-    <t>Ilya Kuryakin</t>
-  </si>
-  <si>
-    <t>Abstract views on foiling the schemes of evil villains</t>
-  </si>
-  <si>
-    <t>Jack Donaghy</t>
-  </si>
-  <si>
-    <t>running a business empire</t>
-  </si>
-  <si>
-    <t>Abstract views on running a business empire</t>
-  </si>
-  <si>
-    <t>Xena</t>
-  </si>
-  <si>
-    <t>fighting for justice</t>
-  </si>
-  <si>
-    <t>Abstract views on fighting for justice</t>
-  </si>
-  <si>
-    <t>Jerry Lee Lewis</t>
-  </si>
-  <si>
-    <t>playing rock piano</t>
-  </si>
-  <si>
-    <t>marrying underage girls</t>
-  </si>
-  <si>
-    <t>George Soros</t>
-  </si>
-  <si>
-    <t>managing hedge funds</t>
-  </si>
-  <si>
-    <t>making billions</t>
-  </si>
-  <si>
-    <t>Abstract views on managing hedge funds</t>
-  </si>
-  <si>
-    <t>Clarice Starling</t>
-  </si>
-  <si>
-    <t>hunting serial killers</t>
-  </si>
-  <si>
-    <t>Abstract views on hunting serial killers</t>
-  </si>
-  <si>
-    <t>Modesty Blaise</t>
-  </si>
-  <si>
-    <t>pulling capers</t>
-  </si>
-  <si>
-    <t>Abstract views on pulling capers</t>
-  </si>
-  <si>
-    <t>Bear Grylls</t>
-  </si>
-  <si>
-    <t>eating bugs</t>
-  </si>
-  <si>
-    <t>licking frogs</t>
-  </si>
-  <si>
-    <t>sucking roots</t>
-  </si>
-  <si>
-    <t>Freddie Mercury</t>
-  </si>
-  <si>
-    <t>singing pop songs</t>
-  </si>
-  <si>
-    <t>writing pop songs</t>
-  </si>
-  <si>
-    <t>cross-dressing in women's clothes</t>
-  </si>
-  <si>
-    <t>Harvey Weinstein</t>
-  </si>
-  <si>
-    <t>chasing after women</t>
-  </si>
-  <si>
-    <t>seducing women</t>
-  </si>
-  <si>
-    <t>making movies</t>
-  </si>
-  <si>
-    <t>Thomas Aquinas</t>
-  </si>
-  <si>
-    <t>Abstract views on teaching philosophy</t>
-  </si>
-  <si>
-    <t>Emmanuel Macron</t>
-  </si>
-  <si>
-    <t>campaigning for the presidency</t>
-  </si>
-  <si>
-    <t>giving speeches</t>
-  </si>
-  <si>
-    <t>Abstract views on campaigning for the presidency</t>
-  </si>
-  <si>
-    <t>Dr. Greg House</t>
-  </si>
-  <si>
-    <t>solving mysteries</t>
-  </si>
-  <si>
-    <t>treating diseases</t>
-  </si>
-  <si>
-    <t>diagnosing diseases</t>
-  </si>
-  <si>
-    <t>finding clues</t>
-  </si>
-  <si>
-    <t>interpreting evidence</t>
-  </si>
-  <si>
-    <t>twirling a cane</t>
-  </si>
-  <si>
-    <t>John McEnroe</t>
-  </si>
-  <si>
-    <t>whining at umpires</t>
-  </si>
-  <si>
-    <t>delivering forehand slams</t>
-  </si>
-  <si>
-    <t>winning tennis tournaments</t>
-  </si>
-  <si>
-    <t>Don King</t>
-  </si>
-  <si>
-    <t>promoting boxing fights</t>
-  </si>
-  <si>
-    <t>Abstract views on promoting boxing fights</t>
-  </si>
-  <si>
-    <t>Benito Mussolini</t>
-  </si>
-  <si>
-    <t>promoting Fascism</t>
-  </si>
-  <si>
-    <t>making trains run on time</t>
-  </si>
-  <si>
-    <t>Abstract views on promoting Fascism</t>
+    <t>punishing criminals</t>
+  </si>
+  <si>
+    <t>undermining authority</t>
+  </si>
+  <si>
+    <t>making vulgar jokes,</t>
+  </si>
+  <si>
+    <t>Polonius</t>
+  </si>
+  <si>
+    <t>coining sententious maxims</t>
+  </si>
+  <si>
+    <t>offering bad advice</t>
+  </si>
+  <si>
+    <t>Abstract views on coining sententious maxims</t>
+  </si>
+  <si>
+    <t>Tim Burton</t>
+  </si>
+  <si>
+    <t>making bizarre movies,</t>
+  </si>
+  <si>
+    <t>Abstract views on making bizarre movies,</t>
+  </si>
+  <si>
+    <t>Dan Brown</t>
+  </si>
+  <si>
+    <t>writing pot-boilers</t>
+  </si>
+  <si>
+    <t>Abstract views on writing pot-boilers</t>
+  </si>
+  <si>
+    <t>Muhammad Ali</t>
+  </si>
+  <si>
+    <t>winning heavyweight titles</t>
+  </si>
+  <si>
+    <t>knocking out opponents</t>
+  </si>
+  <si>
+    <t>winning boxing matches</t>
+  </si>
+  <si>
+    <t>Mr. Darcy</t>
+  </si>
+  <si>
+    <t>looking for love</t>
+  </si>
+  <si>
+    <t>wooing potential brides</t>
+  </si>
+  <si>
+    <t>making condescending remarks</t>
+  </si>
+  <si>
+    <t>James Cook</t>
+  </si>
+  <si>
+    <t>opening new markets</t>
+  </si>
+  <si>
+    <t>exploring foreign countries</t>
+  </si>
+  <si>
+    <t>Abstract views on opening new markets</t>
+  </si>
+  <si>
+    <t>Jack The Ripper</t>
+  </si>
+  <si>
+    <t>terrorizing prostitutes</t>
+  </si>
+  <si>
+    <t>eluding authorities</t>
+  </si>
+  <si>
+    <t>slashing victims</t>
+  </si>
+  <si>
+    <t>eluding capture</t>
+  </si>
+  <si>
+    <t>Olive Oyl</t>
+  </si>
+  <si>
+    <t>doing the Charleston</t>
+  </si>
+  <si>
+    <t>Abstract views on doing the Charleston</t>
+  </si>
+  <si>
+    <t>Barbie</t>
+  </si>
+  <si>
+    <t>promoting hair products</t>
+  </si>
+  <si>
+    <t>Abstract views on promoting hair products</t>
+  </si>
+  <si>
+    <t>Jeff Koons</t>
+  </si>
+  <si>
+    <t>making modern art</t>
+  </si>
+  <si>
+    <t>selling modern art</t>
+  </si>
+  <si>
+    <t>making kitsch</t>
+  </si>
+  <si>
+    <t>selling kitsch</t>
   </si>
 </sst>
 </file>
@@ -410,14 +431,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C87"/>
+  <dimension ref="A1:C92"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="19.44140625" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="47.1640625" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="18.90234375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="44.82421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="15.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -451,73 +472,73 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B8" t="s">
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B9" t="s">
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="10">
@@ -528,7 +549,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11">
@@ -539,7 +560,7 @@
         <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12">
@@ -550,7 +571,7 @@
         <v>20</v>
       </c>
       <c r="C12" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="13">
@@ -572,7 +593,7 @@
         <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
@@ -583,62 +604,62 @@
         <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
+        <v>21</v>
+      </c>
+      <c r="B16" t="s">
         <v>25</v>
       </c>
-      <c r="B16" t="s">
-        <v>26</v>
-      </c>
       <c r="C16" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
+        <v>26</v>
+      </c>
+      <c r="B18" t="s">
         <v>28</v>
       </c>
-      <c r="B18" t="s">
-        <v>29</v>
-      </c>
       <c r="C18" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B20" t="s">
         <v>31</v>
       </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="21">
@@ -649,7 +670,7 @@
         <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="22">
@@ -660,7 +681,7 @@
         <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23">
@@ -671,7 +692,7 @@
         <v>35</v>
       </c>
       <c r="C23" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24">
@@ -679,10 +700,10 @@
         <v>36</v>
       </c>
       <c r="B24" t="s">
-        <v>18</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="25">
@@ -690,117 +711,117 @@
         <v>36</v>
       </c>
       <c r="B25" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
         <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
         <v>41</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29" t="s">
         <v>42</v>
       </c>
-      <c r="B29" t="s">
-        <v>43</v>
-      </c>
       <c r="C29" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B30" t="s">
         <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B31" t="s">
         <v>45</v>
       </c>
       <c r="C31" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" t="s">
         <v>46</v>
       </c>
-      <c r="B32" t="s">
-        <v>47</v>
-      </c>
       <c r="C32" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B33" t="s">
         <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="B34" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="C34" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B35" t="s">
-        <v>51</v>
+        <v>37</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
@@ -808,197 +829,197 @@
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B36" t="s">
-        <v>52</v>
+        <v>40</v>
       </c>
       <c r="C36" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B37" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="C37" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B38" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
       <c r="C38" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B39" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="C39" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B40" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="C40" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="B41" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C41" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>55</v>
       </c>
       <c r="C42" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C43" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="C44" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C45" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B46" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C46" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B47" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
       <c r="C47" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B48" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="C48" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="B49" t="s">
-        <v>39</v>
+        <v>64</v>
       </c>
       <c r="C49" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B50" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C50" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
+        <v>65</v>
+      </c>
+      <c r="B51" t="s">
         <v>67</v>
       </c>
-      <c r="B51" t="s">
-        <v>69</v>
-      </c>
       <c r="C51" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="B52" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C52" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
+        <v>69</v>
+      </c>
+      <c r="B53" t="s">
         <v>70</v>
-      </c>
-      <c r="B53" t="s">
-        <v>72</v>
       </c>
       <c r="C53" t="s">
         <v>5</v>
@@ -1006,10 +1027,10 @@
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B54" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C54" t="s">
         <v>5</v>
@@ -1017,68 +1038,68 @@
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B55" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C55" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>72</v>
+      </c>
+      <c r="B56" t="s">
         <v>74</v>
       </c>
-      <c r="B56" t="s">
-        <v>76</v>
-      </c>
       <c r="C56" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B57" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="C57" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
+        <v>76</v>
+      </c>
+      <c r="B58" t="s">
         <v>77</v>
       </c>
-      <c r="B58" t="s">
-        <v>79</v>
-      </c>
       <c r="C58" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B59" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="C59" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B60" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="C60" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="61">
@@ -1086,7 +1107,7 @@
         <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C61" t="s">
         <v>5</v>
@@ -1094,10 +1115,10 @@
     </row>
     <row r="62">
       <c r="A62" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B62" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="C62" t="s">
         <v>5</v>
@@ -1105,21 +1126,21 @@
     </row>
     <row r="63">
       <c r="A63" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B63" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C63" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
+        <v>80</v>
+      </c>
+      <c r="B64" t="s">
         <v>84</v>
-      </c>
-      <c r="B64" t="s">
-        <v>87</v>
       </c>
       <c r="C64" t="s">
         <v>5</v>
@@ -1127,57 +1148,57 @@
     </row>
     <row r="65">
       <c r="A65" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B65" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="B66" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
+        <v>85</v>
+      </c>
+      <c r="B67" t="s">
         <v>88</v>
       </c>
-      <c r="B67" t="s">
-        <v>91</v>
-      </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B68" t="s">
-        <v>9</v>
+        <v>90</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B69" t="s">
-        <v>10</v>
+        <v>91</v>
       </c>
       <c r="C69" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="70">
@@ -1188,161 +1209,161 @@
         <v>93</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
+        <v>92</v>
+      </c>
+      <c r="B71" t="s">
         <v>94</v>
       </c>
-      <c r="B71" t="s">
-        <v>95</v>
-      </c>
       <c r="C71" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
         <v>96</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B73" t="s">
         <v>97</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
+        <v>95</v>
+      </c>
+      <c r="B74" t="s">
         <v>98</v>
       </c>
-      <c r="B74" t="s">
-        <v>99</v>
-      </c>
       <c r="C74" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B75" t="s">
         <v>100</v>
       </c>
       <c r="C75" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B76" t="s">
         <v>101</v>
       </c>
       <c r="C76" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B77" t="s">
         <v>102</v>
       </c>
       <c r="C77" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B78" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C78" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="B79" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C79" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B80" t="s">
         <v>106</v>
       </c>
       <c r="C80" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B81" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C81" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B82" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B83" t="s">
         <v>110</v>
       </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B84" t="s">
         <v>111</v>
       </c>
       <c r="C84" t="s">
-        <v>5</v>
+        <v>11</v>
       </c>
     </row>
     <row r="85">
@@ -1353,7 +1374,7 @@
         <v>113</v>
       </c>
       <c r="C85" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="86">
@@ -1369,13 +1390,68 @@
     </row>
     <row r="87">
       <c r="A87" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B87" t="s">
+        <v>116</v>
+      </c>
+      <c r="C87" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="s">
         <v>115</v>
       </c>
-      <c r="C87" t="s">
-        <v>5</v>
+      <c r="B88" t="s">
+        <v>117</v>
+      </c>
+      <c r="C88" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="s">
+        <v>118</v>
+      </c>
+      <c r="B89" t="s">
+        <v>119</v>
+      </c>
+      <c r="C89" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="s">
+        <v>118</v>
+      </c>
+      <c r="B90" t="s">
+        <v>120</v>
+      </c>
+      <c r="C90" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="s">
+        <v>118</v>
+      </c>
+      <c r="B91" t="s">
+        <v>121</v>
+      </c>
+      <c r="C91" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="s">
+        <v>118</v>
+      </c>
+      <c r="B92" t="s">
+        <v>122</v>
+      </c>
+      <c r="C92" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit:  Multiple changes made to accommodate for self specified projects
</commit_message>
<xml_diff>
--- a/Staff&Projects(60).xlsx
+++ b/Staff&Projects(60).xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="118">
   <si>
     <t>Supervisor</t>
   </si>
@@ -23,106 +23,193 @@
     <t>Target Audience</t>
   </si>
   <si>
-    <t>Dominique Strauss-Kahn</t>
-  </si>
-  <si>
-    <t>throwing sex parties</t>
+    <t>Rainier Luftwaffe Wolfcastle</t>
+  </si>
+  <si>
+    <t>making action movies</t>
+  </si>
+  <si>
+    <t>DS</t>
+  </si>
+  <si>
+    <t>starring in action movies</t>
+  </si>
+  <si>
+    <t>Abstract views on making action movies</t>
+  </si>
+  <si>
+    <t>Bobby Fischer</t>
+  </si>
+  <si>
+    <t>playing aggressive chess</t>
   </si>
   <si>
     <t>CS + DS</t>
   </si>
   <si>
-    <t>planning orgies</t>
+    <t>Abstract views on playing aggressive chess</t>
   </si>
   <si>
     <t>CS</t>
   </si>
   <si>
-    <t>Abstract views on throwing sex parties</t>
-  </si>
-  <si>
-    <t>Bernard Madoff</t>
-  </si>
-  <si>
-    <t>cheating clients</t>
-  </si>
-  <si>
-    <t>running Ponzi schemes</t>
-  </si>
-  <si>
-    <t>running pyramid schemes</t>
-  </si>
-  <si>
-    <t>Lindsay Lohan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> driving under the influence</t>
-  </si>
-  <si>
-    <t xml:space="preserve">starring in Hollywood movies </t>
-  </si>
-  <si>
-    <t>Abstract views on  driving under the influence</t>
-  </si>
-  <si>
-    <t>Jerry Springer</t>
-  </si>
-  <si>
-    <t>hosting reality TV shows</t>
-  </si>
-  <si>
-    <t>Abstract views on hosting reality TV shows</t>
-  </si>
-  <si>
-    <t>Cary Grant</t>
-  </si>
-  <si>
-    <t>starring in romantic comedies</t>
-  </si>
-  <si>
-    <t>Abstract views on starring in romantic comedies</t>
-  </si>
-  <si>
-    <t>Janis Joplin</t>
-  </si>
-  <si>
-    <t>singing rock songs</t>
-  </si>
-  <si>
-    <t>Abstract views on singing rock songs</t>
-  </si>
-  <si>
-    <t>Mr. Darcy</t>
-  </si>
-  <si>
-    <t>looking for love</t>
-  </si>
-  <si>
-    <t>DS</t>
-  </si>
-  <si>
-    <t>wooing potential brides</t>
-  </si>
-  <si>
-    <t>making condescending remarks</t>
-  </si>
-  <si>
-    <t>Elvis Presley</t>
-  </si>
-  <si>
-    <t>gyrating hips</t>
-  </si>
-  <si>
-    <t>frying peanut-butter and banana sandwiches</t>
-  </si>
-  <si>
-    <t>Juliet Capulet</t>
-  </si>
-  <si>
-    <t>watching the sun rise</t>
-  </si>
-  <si>
-    <t>Abstract views on watching the sun rise</t>
+    <t>Bob Woodward</t>
+  </si>
+  <si>
+    <t>reporting the news</t>
+  </si>
+  <si>
+    <t>following the money</t>
+  </si>
+  <si>
+    <t>Abstract views on reporting the news</t>
+  </si>
+  <si>
+    <t>Beetlejuice</t>
+  </si>
+  <si>
+    <t>practicing the Occult</t>
+  </si>
+  <si>
+    <t>causing mayhem</t>
+  </si>
+  <si>
+    <t>laughing maniacally</t>
+  </si>
+  <si>
+    <t>Holly Golightly</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> climbing social ladders</t>
+  </si>
+  <si>
+    <t>Abstract views on  climbing social ladders</t>
+  </si>
+  <si>
+    <t>Janet Jackson</t>
+  </si>
+  <si>
+    <t>singing pop songs</t>
+  </si>
+  <si>
+    <t>writing pop songs</t>
+  </si>
+  <si>
+    <t>Abstract views on singing pop songs</t>
+  </si>
+  <si>
+    <t>Rocky Balboa</t>
+  </si>
+  <si>
+    <t>winning heavyweight titles</t>
+  </si>
+  <si>
+    <t>knocking out opponents</t>
+  </si>
+  <si>
+    <t>winning boxing matches</t>
+  </si>
+  <si>
+    <t>Saint Peter</t>
+  </si>
+  <si>
+    <t>promoting conservative values</t>
+  </si>
+  <si>
+    <t>Abstract views on promoting conservative values</t>
+  </si>
+  <si>
+    <t>Chewbacca</t>
+  </si>
+  <si>
+    <t>piloting the Millenium Falcon</t>
+  </si>
+  <si>
+    <t>doing the Kessel run</t>
+  </si>
+  <si>
+    <t>smuggling contraband</t>
+  </si>
+  <si>
+    <t>fighting for the rebel alliance</t>
+  </si>
+  <si>
+    <t>piloting a spaceship</t>
+  </si>
+  <si>
+    <t>Deep Throat</t>
+  </si>
+  <si>
+    <t>talking in riddles</t>
+  </si>
+  <si>
+    <t>offering advice</t>
+  </si>
+  <si>
+    <t>Abstract views on talking in riddles</t>
+  </si>
+  <si>
+    <t>Richie Rich</t>
+  </si>
+  <si>
+    <t>squandering money</t>
+  </si>
+  <si>
+    <t>enjoying money</t>
+  </si>
+  <si>
+    <t>Abstract views on squandering money</t>
+  </si>
+  <si>
+    <t>Amy Schumer</t>
+  </si>
+  <si>
+    <t>making vulgar jokes</t>
+  </si>
+  <si>
+    <t>starring in comedies</t>
+  </si>
+  <si>
+    <t>doing stand-up</t>
+  </si>
+  <si>
+    <t>Jean-Paul Sartre</t>
+  </si>
+  <si>
+    <t>popping amphetamines</t>
+  </si>
+  <si>
+    <t>smoking Boyard cigarettes</t>
+  </si>
+  <si>
+    <t>chain-smoking Gauloises Bleues</t>
+  </si>
+  <si>
+    <t>Jason Bourne</t>
+  </si>
+  <si>
+    <t>eluding capture</t>
+  </si>
+  <si>
+    <t>killing people in ingenious ways</t>
+  </si>
+  <si>
+    <t>eluding the CIA</t>
+  </si>
+  <si>
+    <t>Jack Bauer</t>
+  </si>
+  <si>
+    <t>chasing terrorists</t>
+  </si>
+  <si>
+    <t>punishing terrorists</t>
+  </si>
+  <si>
+    <t>tracking down terrorists</t>
+  </si>
+  <si>
+    <t>preventing terrorism</t>
   </si>
   <si>
     <t>George Orwell</t>
@@ -140,223 +227,145 @@
     <t>writing polemics</t>
   </si>
   <si>
-    <t>Tom Cruise</t>
+    <t>Professor Hans Zarkov</t>
+  </si>
+  <si>
+    <t>building rocket ships</t>
+  </si>
+  <si>
+    <t>Abstract views on building rocket ships</t>
+  </si>
+  <si>
+    <t>Bjork</t>
+  </si>
+  <si>
+    <t>Abstract views on writing pop songs</t>
+  </si>
+  <si>
+    <t>Leon Trotsky</t>
+  </si>
+  <si>
+    <t>wielding political power</t>
+  </si>
+  <si>
+    <t>promoting communism</t>
+  </si>
+  <si>
+    <t>launching cultural revolutions</t>
+  </si>
+  <si>
+    <t>Kim Kardashian</t>
+  </si>
+  <si>
+    <t>starring in reality TV shows</t>
+  </si>
+  <si>
+    <t>flaunting buttocks</t>
+  </si>
+  <si>
+    <t>Abstract views on starring in reality TV shows</t>
+  </si>
+  <si>
+    <t>Michael Jordan</t>
+  </si>
+  <si>
+    <t>playing basketball</t>
+  </si>
+  <si>
+    <t>making dunk shots</t>
+  </si>
+  <si>
+    <t>Abstract views on playing basketball</t>
+  </si>
+  <si>
+    <t>Virginia Woolf</t>
+  </si>
+  <si>
+    <t>writing modern fiction</t>
+  </si>
+  <si>
+    <t>Abstract views on writing modern fiction</t>
+  </si>
+  <si>
+    <t>Lee Marvin</t>
   </si>
   <si>
     <t>starring in Hollywood movies</t>
   </si>
   <si>
-    <t>promoting Scientology</t>
-  </si>
-  <si>
-    <t>jumping on couches</t>
-  </si>
-  <si>
-    <t>Saul Goodman</t>
-  </si>
-  <si>
-    <t>protecting criminals</t>
-  </si>
-  <si>
-    <t>representing criminals</t>
-  </si>
-  <si>
-    <t>bending the law</t>
-  </si>
-  <si>
-    <t>offering legal advice</t>
-  </si>
-  <si>
-    <t>Francis Crick</t>
-  </si>
-  <si>
-    <t>studying genetics</t>
-  </si>
-  <si>
-    <t>modeling DNA</t>
-  </si>
-  <si>
-    <t>Abstract views on studying genetics</t>
-  </si>
-  <si>
-    <t>Alexander Fleming</t>
+    <t>playing tough guys</t>
+  </si>
+  <si>
+    <t>Abstract views on starring in Hollywood movies</t>
+  </si>
+  <si>
+    <t>Amelia Earhart</t>
+  </si>
+  <si>
+    <t>flying airplanes</t>
+  </si>
+  <si>
+    <t>breaking records</t>
+  </si>
+  <si>
+    <t>Abstract views on flying airplanes</t>
+  </si>
+  <si>
+    <t>Luciano Pavarotti</t>
+  </si>
+  <si>
+    <t>singing opera arias</t>
+  </si>
+  <si>
+    <t>Abstract views on singing opera arias</t>
+  </si>
+  <si>
+    <t>Sterling Archer</t>
+  </si>
+  <si>
+    <t>going on commando missions</t>
+  </si>
+  <si>
+    <t>kicking ass</t>
+  </si>
+  <si>
+    <t>performing kung-fu moves</t>
+  </si>
+  <si>
+    <t>Wayne Gretzky</t>
+  </si>
+  <si>
+    <t>playing ice hockey</t>
+  </si>
+  <si>
+    <t>Abstract views on playing ice hockey</t>
+  </si>
+  <si>
+    <t>Kal El</t>
+  </si>
+  <si>
+    <t>Stephen Hawking</t>
+  </si>
+  <si>
+    <t>promoting science</t>
   </si>
   <si>
     <t>studying science</t>
   </si>
   <si>
-    <t>Abstract views on studying science</t>
-  </si>
-  <si>
-    <t>Larry King</t>
-  </si>
-  <si>
-    <t>interviewing celebrities</t>
-  </si>
-  <si>
-    <t>interviewing politicians</t>
-  </si>
-  <si>
-    <t>Abstract views on interviewing celebrities</t>
-  </si>
-  <si>
-    <t>Antonio Salieri</t>
-  </si>
-  <si>
-    <t>composing classical music</t>
-  </si>
-  <si>
-    <t xml:space="preserve">burning with envy </t>
-  </si>
-  <si>
-    <t>Abstract views on composing classical music</t>
-  </si>
-  <si>
-    <t>Hans Gruber</t>
-  </si>
-  <si>
-    <t>organizing armed robberies</t>
-  </si>
-  <si>
-    <t>Abstract views on organizing armed robberies</t>
-  </si>
-  <si>
-    <t>Professor James Moriarty</t>
-  </si>
-  <si>
-    <t>plotting criminal schemes</t>
-  </si>
-  <si>
-    <t>amassing ill-gotten wealth</t>
-  </si>
-  <si>
-    <t>Abstract views on plotting criminal schemes</t>
-  </si>
-  <si>
-    <t>Mad Max Rockatansky</t>
-  </si>
-  <si>
-    <t>avenging loved ones</t>
-  </si>
-  <si>
-    <t>surviving in a post-apocalyptic world</t>
-  </si>
-  <si>
-    <t>defending the weak</t>
-  </si>
-  <si>
-    <t>Caitlyn Jenner</t>
-  </si>
-  <si>
-    <t>campaigning for social causes</t>
-  </si>
-  <si>
-    <t>Abstract views on campaigning for social causes</t>
-  </si>
-  <si>
-    <t>Dr. John Watson</t>
-  </si>
-  <si>
-    <t>chasing criminals</t>
-  </si>
-  <si>
-    <t>offering medical opinions</t>
-  </si>
-  <si>
-    <t>writing up case notes</t>
-  </si>
-  <si>
-    <t>Eddie Murphy</t>
-  </si>
-  <si>
-    <t>starring in action movies</t>
-  </si>
-  <si>
-    <t>starring in comedies</t>
-  </si>
-  <si>
-    <t>Abstract views on starring in action movies</t>
-  </si>
-  <si>
-    <t>Clint Eastwood</t>
-  </si>
-  <si>
-    <t>directing movies</t>
-  </si>
-  <si>
-    <t>Frank Capra</t>
-  </si>
-  <si>
-    <t>making idealistic movies</t>
-  </si>
-  <si>
-    <t>Abstract views on making idealistic movies</t>
-  </si>
-  <si>
-    <t>Johann von Goethe</t>
-  </si>
-  <si>
-    <t>writing poetry</t>
-  </si>
-  <si>
-    <t>writing about social problems,</t>
-  </si>
-  <si>
-    <t>Abstract views on writing poetry</t>
-  </si>
-  <si>
-    <t>George Armstrong Custer</t>
-  </si>
-  <si>
-    <t>developing military strategies</t>
-  </si>
-  <si>
-    <t>leading armies into battle</t>
-  </si>
-  <si>
-    <t>Abstract views on developing military strategies</t>
-  </si>
-  <si>
-    <t>Samwise Gamgee</t>
-  </si>
-  <si>
-    <t>tending the garden</t>
-  </si>
-  <si>
-    <t>planting daffodils</t>
-  </si>
-  <si>
-    <t>cooking a rabbit stew</t>
-  </si>
-  <si>
-    <t>Stan Lee</t>
-  </si>
-  <si>
-    <t>writing comic books</t>
-  </si>
-  <si>
-    <t>inventing superheroes</t>
-  </si>
-  <si>
-    <t>Abstract views on writing comic books</t>
-  </si>
-  <si>
-    <t>Frank Gehry</t>
-  </si>
-  <si>
-    <t>designing modern buildings</t>
-  </si>
-  <si>
-    <t>Abstract views on designing modern buildings</t>
-  </si>
-  <si>
-    <t>Iggy Pop</t>
-  </si>
-  <si>
-    <t>doing raunchy stage acts</t>
-  </si>
-  <si>
-    <t>Abstract views on doing raunchy stage acts</t>
+    <t>transcending physical limits</t>
+  </si>
+  <si>
+    <t>King Solomon</t>
+  </si>
+  <si>
+    <t>ruling over subjects</t>
+  </si>
+  <si>
+    <t>running a kingdom</t>
+  </si>
+  <si>
+    <t>Abstract views on ruling over subjects</t>
   </si>
 </sst>
 </file>
@@ -407,14 +416,14 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C87"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="23.875" customWidth="true" bestFit="true"/>
-    <col min="2" max="2" width="44.046875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="26.3359375" customWidth="true" bestFit="true"/>
+    <col min="2" max="2" width="44.82421875" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="15.9765625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -448,7 +457,7 @@
         <v>6</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -456,7 +465,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
@@ -464,35 +473,35 @@
     </row>
     <row r="5">
       <c r="A5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
-        <v>10</v>
-      </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="B7" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8">
@@ -500,10 +509,10 @@
         <v>13</v>
       </c>
       <c r="B8" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9">
@@ -511,21 +520,21 @@
         <v>13</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B10" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="11">
@@ -533,10 +542,10 @@
         <v>17</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12">
@@ -544,7 +553,7 @@
         <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -552,10 +561,10 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B13" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
@@ -563,109 +572,109 @@
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B14" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C14" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C16" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
         <v>27</v>
       </c>
       <c r="C17" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
         <v>29</v>
       </c>
       <c r="C18" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B20" t="s">
         <v>31</v>
       </c>
-      <c r="B20" t="s">
-        <v>24</v>
-      </c>
       <c r="C20" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B21" t="s">
-        <v>21</v>
+        <v>33</v>
       </c>
       <c r="C21" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="C22" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="B23" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C23" t="s">
         <v>5</v>
@@ -673,87 +682,87 @@
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="C24" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B25" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="C25" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B26" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C26" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B27" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B28" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="C28" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B29" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C29" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C30" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B31" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C31" t="s">
         <v>5</v>
@@ -761,10 +770,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B32" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C32" t="s">
         <v>5</v>
@@ -772,109 +781,109 @@
     </row>
     <row r="33">
       <c r="A33" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B33" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C33" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B34" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C34" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B35" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="C35" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="B36" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="C36" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B37" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="C37" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B38" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="C38" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B39" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="C39" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B40" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="C40" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="C41" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B42" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C42" t="s">
         <v>5</v>
@@ -882,10 +891,10 @@
     </row>
     <row r="43">
       <c r="A43" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B43" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="C43" t="s">
         <v>5</v>
@@ -893,21 +902,21 @@
     </row>
     <row r="44">
       <c r="A44" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B44" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="C44" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="C45" t="s">
         <v>5</v>
@@ -915,10 +924,10 @@
     </row>
     <row r="46">
       <c r="A46" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C46" t="s">
         <v>5</v>
@@ -926,13 +935,13 @@
     </row>
     <row r="47">
       <c r="A47" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="B47" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="C47" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="48">
@@ -940,10 +949,10 @@
         <v>66</v>
       </c>
       <c r="B48" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="C48" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49">
@@ -951,109 +960,109 @@
         <v>66</v>
       </c>
       <c r="B49" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C49" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B50" t="s">
         <v>70</v>
       </c>
       <c r="C50" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B51" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C51" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B52" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="C52" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B53" t="s">
-        <v>74</v>
+        <v>26</v>
       </c>
       <c r="C53" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B54" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="C54" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C55" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s">
+        <v>76</v>
+      </c>
+      <c r="B56" t="s">
         <v>77</v>
       </c>
-      <c r="B56" t="s">
-        <v>78</v>
-      </c>
       <c r="C56" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B57" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C57" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B58" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C58" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="59">
@@ -1061,10 +1070,10 @@
         <v>80</v>
       </c>
       <c r="B59" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C59" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
     </row>
     <row r="60">
@@ -1072,21 +1081,21 @@
         <v>80</v>
       </c>
       <c r="B60" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C60" t="s">
-        <v>28</v>
+        <v>12</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="B61" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C61" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="62">
@@ -1094,10 +1103,10 @@
         <v>84</v>
       </c>
       <c r="B62" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C62" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="63">
@@ -1105,21 +1114,21 @@
         <v>84</v>
       </c>
       <c r="B63" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C63" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="B64" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="C64" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="65">
@@ -1130,7 +1139,7 @@
         <v>89</v>
       </c>
       <c r="C65" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="66">
@@ -1138,161 +1147,161 @@
         <v>88</v>
       </c>
       <c r="B66" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="C66" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B67" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="C67" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B68" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C68" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B69" t="s">
         <v>94</v>
       </c>
       <c r="C69" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B70" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C70" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B71" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C71" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B72" t="s">
         <v>98</v>
       </c>
       <c r="C72" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C73" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C74" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B75" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="C75" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B76" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C76" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B77" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="C77" t="s">
-        <v>28</v>
+        <v>5</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B78" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C78" t="s">
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B79" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C79" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s">
-        <v>105</v>
+        <v>109</v>
       </c>
       <c r="B80" t="s">
-        <v>108</v>
+        <v>14</v>
       </c>
       <c r="C80" t="s">
         <v>5</v>
@@ -1303,43 +1312,76 @@
         <v>109</v>
       </c>
       <c r="B81" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="C81" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B82" t="s">
         <v>111</v>
       </c>
       <c r="C82" t="s">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s">
+        <v>110</v>
+      </c>
+      <c r="B83" t="s">
         <v>112</v>
       </c>
-      <c r="B83" t="s">
-        <v>113</v>
-      </c>
       <c r="C83" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="B84" t="s">
+        <v>113</v>
+      </c>
+      <c r="C84" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="s">
         <v>114</v>
       </c>
-      <c r="C84" t="s">
-        <v>7</v>
+      <c r="B85" t="s">
+        <v>115</v>
+      </c>
+      <c r="C85" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="s">
+        <v>114</v>
+      </c>
+      <c r="B86" t="s">
+        <v>116</v>
+      </c>
+      <c r="C86" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="s">
+        <v>114</v>
+      </c>
+      <c r="B87" t="s">
+        <v>117</v>
+      </c>
+      <c r="C87" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>